<commit_message>
Updated documents in FasiTahir branch
</commit_message>
<xml_diff>
--- a/Documents/Kickoff_User_Story.xlsx
+++ b/Documents/Kickoff_User_Story.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FasiTahir\6th Semester\SPM\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240A655C-2EE5-41D5-8BC5-2C3DC7063115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9304FD54-81A9-4E7E-9AC6-812BC55E294F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="113">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -361,6 +361,12 @@
   <si>
     <t>Dr. Khaldoon Khurshid</t>
   </si>
+  <si>
+    <t>Assign teachers to courses and sections</t>
+  </si>
+  <si>
+    <t>Manage the teaching assignments effectively</t>
+  </si>
 </sst>
 </file>
 
@@ -559,7 +565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -601,6 +607,27 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -622,26 +649,11 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -712,9 +724,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -752,7 +764,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -858,7 +870,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1000,7 +1012,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1010,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AZ410"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="96" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="96" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1044,12 +1056,12 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -1063,11 +1075,11 @@
       <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -1079,11 +1091,11 @@
       <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -1144,7 +1156,7 @@
     </row>
     <row r="6" spans="1:52" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="3"/>
@@ -1208,7 +1220,7 @@
     </row>
     <row r="7" spans="1:52" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="21"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="3"/>
       <c r="D7" s="12">
         <v>1</v>
@@ -1270,7 +1282,7 @@
     </row>
     <row r="8" spans="1:52" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="29" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="3"/>
@@ -1334,7 +1346,7 @@
     </row>
     <row r="9" spans="1:52" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="23"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="3"/>
       <c r="D9" s="12">
         <v>3</v>
@@ -1396,7 +1408,7 @@
     </row>
     <row r="10" spans="1:52" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="23"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="3"/>
       <c r="D10" s="13">
         <v>4</v>
@@ -1458,7 +1470,7 @@
     </row>
     <row r="11" spans="1:52" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="23"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="3"/>
       <c r="D11" s="12">
         <v>5</v>
@@ -3886,13 +3898,13 @@
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
-      <c r="D50" s="25">
+      <c r="D50" s="18">
         <v>44</v>
       </c>
-      <c r="E50" s="27" t="s">
+      <c r="E50" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="F50" s="30" t="s">
+      <c r="F50" s="23" t="s">
         <v>97</v>
       </c>
       <c r="G50" s="16" t="s">
@@ -3948,16 +3960,16 @@
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
-      <c r="D51" s="26">
+      <c r="D51" s="19">
         <v>45</v>
       </c>
-      <c r="E51" s="28" t="s">
+      <c r="E51" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="F51" s="28" t="s">
+      <c r="F51" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="G51" s="24" t="s">
+      <c r="G51" s="17" t="s">
         <v>98</v>
       </c>
       <c r="H51" s="3"/>
@@ -4010,13 +4022,13 @@
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
-      <c r="D52" s="25">
+      <c r="D52" s="18">
         <v>46</v>
       </c>
-      <c r="E52" s="29" t="s">
+      <c r="E52" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F52" s="29" t="s">
+      <c r="F52" s="22" t="s">
         <v>100</v>
       </c>
       <c r="G52" s="15" t="s">
@@ -4068,11 +4080,19 @@
       <c r="AY52" s="1"/>
       <c r="AZ52" s="1"/>
     </row>
-    <row r="53" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
+    <row r="53" spans="1:52" ht="30" x14ac:dyDescent="0.25">
+      <c r="D53" s="19">
+        <v>47</v>
+      </c>
+      <c r="E53" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F53" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G53" s="32" t="s">
+        <v>112</v>
+      </c>
       <c r="H53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
@@ -21984,24 +22004,24 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22222,6 +22242,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3ADE4A5-5187-46C5-8CDB-A4ADE256890D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD055CC2-8F68-4C69-9E56-54BEA8C803C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -22234,14 +22262,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3ADE4A5-5187-46C5-8CDB-A4ADE256890D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>